<commit_message>
Agente agregado en reporte de Saldos
</commit_message>
<xml_diff>
--- a/reportes/base/osaldoDeudorCliente.xlsx
+++ b/reportes/base/osaldoDeudorCliente.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uemar\Desktop\calera\report_sa_services\reportes\base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B38ECF4D-7C8D-489D-820B-3ADEEE86FFD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{100549B1-D091-42CF-9572-8F49006EE35B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t xml:space="preserve">Saldo deudor del cliente. </t>
   </si>
@@ -59,6 +59,9 @@
   </si>
   <si>
     <t>Fecha:</t>
+  </si>
+  <si>
+    <t>Agente</t>
   </si>
 </sst>
 </file>
@@ -497,69 +500,78 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:H40"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScale="130" zoomScaleNormal="100" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.1796875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="8.08984375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="12.7265625" style="2" customWidth="1"/>
-    <col min="4" max="6" width="14.08984375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="9.1796875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="20.08984375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="20.1796875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="8.08984375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="9.90625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="10.08984375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="10" style="2" customWidth="1"/>
+    <col min="7" max="7" width="10.26953125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="9.1796875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
-    </row>
-    <row r="2" spans="1:7" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="D1" s="10"/>
+    </row>
+    <row r="2" spans="1:8" s="2" customFormat="1" ht="16.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
-      <c r="F2" s="7" t="s">
+      <c r="D2" s="4"/>
+      <c r="G2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="8">
+      <c r="H2" s="8">
         <f ca="1">TODAY()</f>
-        <v>44785</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="6.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>44800</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="6.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-    </row>
-    <row r="4" spans="1:7" s="6" customFormat="1" ht="32" x14ac:dyDescent="0.35">
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" s="6" customFormat="1" ht="32" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="C4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="D4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="E4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="F4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="G4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="H4" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="9"/>
       <c r="B5" s="9"/>
       <c r="C5" s="9"/>
@@ -567,8 +579,9 @@
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
       <c r="G5" s="9"/>
-    </row>
-    <row r="6" spans="1:7" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H5" s="9"/>
+    </row>
+    <row r="6" spans="1:8" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="9"/>
       <c r="B6" s="9"/>
       <c r="C6" s="9"/>
@@ -576,8 +589,9 @@
       <c r="E6" s="9"/>
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
-    </row>
-    <row r="7" spans="1:7" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H6" s="9"/>
+    </row>
+    <row r="7" spans="1:8" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="9"/>
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
@@ -585,8 +599,9 @@
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
-    </row>
-    <row r="8" spans="1:7" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H7" s="9"/>
+    </row>
+    <row r="8" spans="1:8" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="9"/>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
@@ -594,8 +609,9 @@
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
-    </row>
-    <row r="9" spans="1:7" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H8" s="9"/>
+    </row>
+    <row r="9" spans="1:8" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="9"/>
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
@@ -603,8 +619,9 @@
       <c r="E9" s="9"/>
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
-    </row>
-    <row r="10" spans="1:7" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H9" s="9"/>
+    </row>
+    <row r="10" spans="1:8" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="9"/>
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>
@@ -612,8 +629,9 @@
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
-    </row>
-    <row r="11" spans="1:7" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H10" s="9"/>
+    </row>
+    <row r="11" spans="1:8" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="9"/>
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
@@ -621,8 +639,9 @@
       <c r="E11" s="9"/>
       <c r="F11" s="9"/>
       <c r="G11" s="9"/>
-    </row>
-    <row r="12" spans="1:7" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H11" s="9"/>
+    </row>
+    <row r="12" spans="1:8" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="9"/>
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
@@ -630,8 +649,9 @@
       <c r="E12" s="9"/>
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
-    </row>
-    <row r="13" spans="1:7" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H12" s="9"/>
+    </row>
+    <row r="13" spans="1:8" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="9"/>
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
@@ -639,8 +659,9 @@
       <c r="E13" s="9"/>
       <c r="F13" s="9"/>
       <c r="G13" s="9"/>
-    </row>
-    <row r="14" spans="1:7" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H13" s="9"/>
+    </row>
+    <row r="14" spans="1:8" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="9"/>
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
@@ -648,8 +669,9 @@
       <c r="E14" s="9"/>
       <c r="F14" s="9"/>
       <c r="G14" s="9"/>
-    </row>
-    <row r="15" spans="1:7" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H14" s="9"/>
+    </row>
+    <row r="15" spans="1:8" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="9"/>
       <c r="B15" s="9"/>
       <c r="C15" s="9"/>
@@ -657,8 +679,9 @@
       <c r="E15" s="9"/>
       <c r="F15" s="9"/>
       <c r="G15" s="9"/>
-    </row>
-    <row r="16" spans="1:7" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H15" s="9"/>
+    </row>
+    <row r="16" spans="1:8" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="9"/>
       <c r="B16" s="9"/>
       <c r="C16" s="9"/>
@@ -666,8 +689,9 @@
       <c r="E16" s="9"/>
       <c r="F16" s="9"/>
       <c r="G16" s="9"/>
-    </row>
-    <row r="17" spans="1:7" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H16" s="9"/>
+    </row>
+    <row r="17" spans="1:8" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="9"/>
       <c r="B17" s="9"/>
       <c r="C17" s="9"/>
@@ -675,8 +699,9 @@
       <c r="E17" s="9"/>
       <c r="F17" s="9"/>
       <c r="G17" s="9"/>
-    </row>
-    <row r="18" spans="1:7" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H17" s="9"/>
+    </row>
+    <row r="18" spans="1:8" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="9"/>
       <c r="B18" s="9"/>
       <c r="C18" s="9"/>
@@ -684,8 +709,9 @@
       <c r="E18" s="9"/>
       <c r="F18" s="9"/>
       <c r="G18" s="9"/>
-    </row>
-    <row r="19" spans="1:7" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H18" s="9"/>
+    </row>
+    <row r="19" spans="1:8" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="9"/>
       <c r="B19" s="9"/>
       <c r="C19" s="9"/>
@@ -693,8 +719,9 @@
       <c r="E19" s="9"/>
       <c r="F19" s="9"/>
       <c r="G19" s="9"/>
-    </row>
-    <row r="20" spans="1:7" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H19" s="9"/>
+    </row>
+    <row r="20" spans="1:8" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="9"/>
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
@@ -702,8 +729,9 @@
       <c r="E20" s="9"/>
       <c r="F20" s="9"/>
       <c r="G20" s="9"/>
-    </row>
-    <row r="21" spans="1:7" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H20" s="9"/>
+    </row>
+    <row r="21" spans="1:8" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="9"/>
       <c r="B21" s="9"/>
       <c r="C21" s="9"/>
@@ -711,8 +739,9 @@
       <c r="E21" s="9"/>
       <c r="F21" s="9"/>
       <c r="G21" s="9"/>
-    </row>
-    <row r="22" spans="1:7" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H21" s="9"/>
+    </row>
+    <row r="22" spans="1:8" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="9"/>
       <c r="B22" s="9"/>
       <c r="C22" s="9"/>
@@ -720,8 +749,9 @@
       <c r="E22" s="9"/>
       <c r="F22" s="9"/>
       <c r="G22" s="9"/>
-    </row>
-    <row r="23" spans="1:7" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H22" s="9"/>
+    </row>
+    <row r="23" spans="1:8" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="9"/>
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
@@ -729,8 +759,9 @@
       <c r="E23" s="9"/>
       <c r="F23" s="9"/>
       <c r="G23" s="9"/>
-    </row>
-    <row r="24" spans="1:7" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H23" s="9"/>
+    </row>
+    <row r="24" spans="1:8" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="9"/>
       <c r="B24" s="9"/>
       <c r="C24" s="9"/>
@@ -738,8 +769,9 @@
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
-    </row>
-    <row r="25" spans="1:7" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H24" s="9"/>
+    </row>
+    <row r="25" spans="1:8" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="9"/>
       <c r="B25" s="9"/>
       <c r="C25" s="9"/>
@@ -747,8 +779,9 @@
       <c r="E25" s="9"/>
       <c r="F25" s="9"/>
       <c r="G25" s="9"/>
-    </row>
-    <row r="26" spans="1:7" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H25" s="9"/>
+    </row>
+    <row r="26" spans="1:8" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="9"/>
       <c r="B26" s="9"/>
       <c r="C26" s="9"/>
@@ -756,8 +789,9 @@
       <c r="E26" s="9"/>
       <c r="F26" s="9"/>
       <c r="G26" s="9"/>
-    </row>
-    <row r="27" spans="1:7" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H26" s="9"/>
+    </row>
+    <row r="27" spans="1:8" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="9"/>
       <c r="B27" s="9"/>
       <c r="C27" s="9"/>
@@ -765,8 +799,9 @@
       <c r="E27" s="9"/>
       <c r="F27" s="9"/>
       <c r="G27" s="9"/>
-    </row>
-    <row r="28" spans="1:7" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H27" s="9"/>
+    </row>
+    <row r="28" spans="1:8" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="9"/>
       <c r="B28" s="9"/>
       <c r="C28" s="9"/>
@@ -774,8 +809,9 @@
       <c r="E28" s="9"/>
       <c r="F28" s="9"/>
       <c r="G28" s="9"/>
-    </row>
-    <row r="29" spans="1:7" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H28" s="9"/>
+    </row>
+    <row r="29" spans="1:8" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="9"/>
       <c r="B29" s="9"/>
       <c r="C29" s="9"/>
@@ -783,8 +819,9 @@
       <c r="E29" s="9"/>
       <c r="F29" s="9"/>
       <c r="G29" s="9"/>
-    </row>
-    <row r="30" spans="1:7" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H29" s="9"/>
+    </row>
+    <row r="30" spans="1:8" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="9"/>
       <c r="B30" s="9"/>
       <c r="C30" s="9"/>
@@ -792,8 +829,9 @@
       <c r="E30" s="9"/>
       <c r="F30" s="9"/>
       <c r="G30" s="9"/>
-    </row>
-    <row r="31" spans="1:7" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H30" s="9"/>
+    </row>
+    <row r="31" spans="1:8" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="9"/>
       <c r="B31" s="9"/>
       <c r="C31" s="9"/>
@@ -801,8 +839,9 @@
       <c r="E31" s="9"/>
       <c r="F31" s="9"/>
       <c r="G31" s="9"/>
-    </row>
-    <row r="32" spans="1:7" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H31" s="9"/>
+    </row>
+    <row r="32" spans="1:8" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="9"/>
       <c r="B32" s="9"/>
       <c r="C32" s="9"/>
@@ -810,8 +849,9 @@
       <c r="E32" s="9"/>
       <c r="F32" s="9"/>
       <c r="G32" s="9"/>
-    </row>
-    <row r="33" spans="1:7" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H32" s="9"/>
+    </row>
+    <row r="33" spans="1:8" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="9"/>
       <c r="B33" s="9"/>
       <c r="C33" s="9"/>
@@ -819,8 +859,9 @@
       <c r="E33" s="9"/>
       <c r="F33" s="9"/>
       <c r="G33" s="9"/>
-    </row>
-    <row r="34" spans="1:7" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H33" s="9"/>
+    </row>
+    <row r="34" spans="1:8" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="9"/>
       <c r="B34" s="9"/>
       <c r="C34" s="9"/>
@@ -828,8 +869,9 @@
       <c r="E34" s="9"/>
       <c r="F34" s="9"/>
       <c r="G34" s="9"/>
-    </row>
-    <row r="35" spans="1:7" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H34" s="9"/>
+    </row>
+    <row r="35" spans="1:8" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="9"/>
       <c r="B35" s="9"/>
       <c r="C35" s="9"/>
@@ -837,8 +879,9 @@
       <c r="E35" s="9"/>
       <c r="F35" s="9"/>
       <c r="G35" s="9"/>
-    </row>
-    <row r="36" spans="1:7" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H35" s="9"/>
+    </row>
+    <row r="36" spans="1:8" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="9"/>
       <c r="B36" s="9"/>
       <c r="C36" s="9"/>
@@ -846,8 +889,9 @@
       <c r="E36" s="9"/>
       <c r="F36" s="9"/>
       <c r="G36" s="9"/>
-    </row>
-    <row r="37" spans="1:7" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H36" s="9"/>
+    </row>
+    <row r="37" spans="1:8" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="9"/>
       <c r="B37" s="9"/>
       <c r="C37" s="9"/>
@@ -855,8 +899,9 @@
       <c r="E37" s="9"/>
       <c r="F37" s="9"/>
       <c r="G37" s="9"/>
-    </row>
-    <row r="38" spans="1:7" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H37" s="9"/>
+    </row>
+    <row r="38" spans="1:8" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="9"/>
       <c r="B38" s="9"/>
       <c r="C38" s="9"/>
@@ -864,8 +909,9 @@
       <c r="E38" s="9"/>
       <c r="F38" s="9"/>
       <c r="G38" s="9"/>
-    </row>
-    <row r="39" spans="1:7" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H38" s="9"/>
+    </row>
+    <row r="39" spans="1:8" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="9"/>
       <c r="B39" s="9"/>
       <c r="C39" s="9"/>
@@ -873,8 +919,9 @@
       <c r="E39" s="9"/>
       <c r="F39" s="9"/>
       <c r="G39" s="9"/>
-    </row>
-    <row r="40" spans="1:7" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H39" s="9"/>
+    </row>
+    <row r="40" spans="1:8" s="2" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
@@ -882,10 +929,11 @@
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
       <c r="G40" s="3"/>
+      <c r="H40" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A1:D1"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>